<commit_message>
updating website to match latest version
</commit_message>
<xml_diff>
--- a/artifacts/MobileCoverage/assets/data/CoverageResults.xlsx
+++ b/artifacts/MobileCoverage/assets/data/CoverageResults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fariakn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fariakn\Research\website\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF0707AA-36BD-467C-BEE5-B9084F5B37D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC191F3-37FE-4D3E-BC07-1D23096A0FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" firstSheet="29" activeTab="31" xr2:uid="{A62121A6-B06E-4EA5-80E6-B92E89DA2E47}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{A62121A6-B06E-4EA5-80E6-B92E89DA2E47}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Coverage" sheetId="43" r:id="rId1"/>
@@ -10900,7 +10900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E013AF-4B40-49A6-9099-67068B933BEF}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -30082,7 +30082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77A204B-6835-4518-9609-7ACD8CEAED77}">
   <dimension ref="A1:E158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>

</xml_diff>